<commit_message>
[Test] test 양식 update - Done
</commit_message>
<xml_diff>
--- a/cafe24 양식/봉지라면_3ea.xlsx
+++ b/cafe24 양식/봉지라면_3ea.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="125">
   <si>
     <t>상품코드</t>
   </si>
@@ -318,20 +318,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>M000000A</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>평일 09:30~17:30
-점심 12:00~13:00
-토,일요일 공휴일 휴무</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;IMG src="http://tongup1emd.cafe24.com/img/Image_detail/notice.jpg" width=860&gt;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>1|16|2500//17|32|5000//33|48|7500//49|64|10000//65|80|12500//81|96|15000</t>
   </si>
   <si>
@@ -364,10 +350,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;IMG src="http://tongup1emd.cafe24.com/img/Image_detail/notice.jpg" width=860&gt;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>&lt;p&gt;&lt;/p&gt;&lt;p align="center"&gt;&lt;IMG src="http://tongup1emd.cafe24.com/img/Image_detail/01_Noodle_68ea/2414_detail.jpg" style="width:860px;"&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
   </si>
   <si>
@@ -375,11 +357,6 @@
   </si>
   <si>
     <t>&lt;p&gt;&lt;/p&gt;&lt;p align="center"&gt;&lt;IMG src="http://tongup1emd.cafe24.com/img/Image_detail/01_Noodle_68ea/2416_detail.jpg" style="width:860px;"&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-</t>
-    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>2414_450x450.jpg</t>
@@ -428,6 +405,9 @@
   <si>
     <t>2416_220x220.jpg</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>M000000E</t>
   </si>
 </sst>
 </file>
@@ -437,7 +417,7 @@
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -614,12 +594,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <name val="돋움"/>
-      <family val="3"/>
-      <charset val="129"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
@@ -840,7 +814,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -985,6 +959,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1139,7 +1128,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
@@ -1160,11 +1149,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1509,10 +1498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CJ10"/>
+  <dimension ref="A1:CJ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BK1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BT16" sqref="BT16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1798,7 +1787,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:88" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:88" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="1">
         <v>2414</v>
@@ -1828,7 +1817,7 @@
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
       <c r="O2" s="8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="P2" s="5" t="s">
         <v>89</v>
@@ -1877,19 +1866,19 @@
       <c r="AR2" s="5"/>
       <c r="AS2" s="5"/>
       <c r="AT2" s="8" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="AU2" s="8" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="AV2" s="8" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="AW2" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="AX2" s="5" t="s">
-        <v>100</v>
+        <v>121</v>
+      </c>
+      <c r="AX2" s="15" t="s">
+        <v>124</v>
       </c>
       <c r="AY2" s="4"/>
       <c r="AZ2" s="5"/>
@@ -1906,13 +1895,9 @@
       </c>
       <c r="BH2" s="5"/>
       <c r="BI2" s="5"/>
-      <c r="BJ2" s="5" t="s">
-        <v>112</v>
-      </c>
+      <c r="BJ2" s="5"/>
       <c r="BK2" s="5"/>
-      <c r="BL2" s="7" t="s">
-        <v>101</v>
-      </c>
+      <c r="BL2" s="7"/>
       <c r="BM2" s="5" t="s">
         <v>91</v>
       </c>
@@ -1931,7 +1916,7 @@
         <v>92</v>
       </c>
       <c r="BT2" s="8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="BU2" s="5"/>
       <c r="BV2" s="5"/>
@@ -1944,23 +1929,23 @@
         <v>88</v>
       </c>
       <c r="CC2" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="CD2" s="5"/>
       <c r="CE2" s="5"/>
       <c r="CF2" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="CG2" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="CG2" s="8" t="s">
+      <c r="CH2" s="5" t="s">
         <v>107</v>
-      </c>
-      <c r="CH2" s="5" t="s">
-        <v>110</v>
       </c>
       <c r="CI2" s="5"/>
       <c r="CJ2" s="5"/>
     </row>
-    <row r="3" spans="1:88" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:88" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="1">
         <v>2415</v>
@@ -1990,7 +1975,7 @@
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
       <c r="O3" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="P3" s="5" t="s">
         <v>89</v>
@@ -2039,19 +2024,19 @@
       <c r="AR3" s="5"/>
       <c r="AS3" s="5"/>
       <c r="AT3" s="8" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="AU3" s="8" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="AV3" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="AW3" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="AX3" s="15" t="s">
         <v>124</v>
-      </c>
-      <c r="AW3" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="AX3" s="5" t="s">
-        <v>100</v>
       </c>
       <c r="AY3" s="4"/>
       <c r="AZ3" s="5"/>
@@ -2068,13 +2053,9 @@
       </c>
       <c r="BH3" s="5"/>
       <c r="BI3" s="5"/>
-      <c r="BJ3" s="5" t="s">
-        <v>102</v>
-      </c>
+      <c r="BJ3" s="5"/>
       <c r="BK3" s="5"/>
-      <c r="BL3" s="7" t="s">
-        <v>101</v>
-      </c>
+      <c r="BL3" s="7"/>
       <c r="BM3" s="5" t="s">
         <v>91</v>
       </c>
@@ -2093,7 +2074,7 @@
         <v>92</v>
       </c>
       <c r="BT3" s="8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="BU3" s="5"/>
       <c r="BV3" s="5"/>
@@ -2106,23 +2087,23 @@
         <v>88</v>
       </c>
       <c r="CC3" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="CD3" s="5"/>
       <c r="CE3" s="5"/>
       <c r="CF3" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="CG3" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="CG3" s="8" t="s">
-        <v>108</v>
-      </c>
       <c r="CH3" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="CI3" s="5"/>
       <c r="CJ3" s="5"/>
     </row>
-    <row r="4" spans="1:88" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:88" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="1">
         <v>2416</v>
@@ -2152,7 +2133,7 @@
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="O4" s="8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="P4" s="5" t="s">
         <v>89</v>
@@ -2201,19 +2182,19 @@
       <c r="AR4" s="5"/>
       <c r="AS4" s="5"/>
       <c r="AT4" s="8" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="AU4" s="8" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="AV4" s="8" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="AW4" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="AX4" s="5" t="s">
-        <v>100</v>
+        <v>123</v>
+      </c>
+      <c r="AX4" s="15" t="s">
+        <v>124</v>
       </c>
       <c r="AY4" s="4"/>
       <c r="AZ4" s="5"/>
@@ -2230,13 +2211,9 @@
       </c>
       <c r="BH4" s="5"/>
       <c r="BI4" s="5"/>
-      <c r="BJ4" s="5" t="s">
-        <v>102</v>
-      </c>
+      <c r="BJ4" s="5"/>
       <c r="BK4" s="5"/>
-      <c r="BL4" s="7" t="s">
-        <v>101</v>
-      </c>
+      <c r="BL4" s="7"/>
       <c r="BM4" s="5" t="s">
         <v>91</v>
       </c>
@@ -2255,7 +2232,7 @@
         <v>92</v>
       </c>
       <c r="BT4" s="8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="BU4" s="5"/>
       <c r="BV4" s="5"/>
@@ -2268,26 +2245,21 @@
         <v>88</v>
       </c>
       <c r="CC4" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="CD4" s="5"/>
       <c r="CE4" s="5"/>
       <c r="CF4" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="CG4" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="CG4" s="8" t="s">
-        <v>109</v>
-      </c>
       <c r="CH4" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="CI4" s="5"/>
       <c r="CJ4" s="5"/>
-    </row>
-    <row r="10" spans="1:88" ht="33" x14ac:dyDescent="0.3">
-      <c r="AT10" s="15" t="s">
-        <v>116</v>
-      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>